<commit_message>
worked on motor drive and balance modules
</commit_message>
<xml_diff>
--- a/time_tracker.xlsx
+++ b/time_tracker.xlsx
@@ -8,29 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Horia\Documents\COEN-6711\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413677BE-1227-4D15-8D33-E8F8FACA6D88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBED8188-424E-48C8-9B99-2BA61FCC385B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +43,12 @@
   </si>
   <si>
     <t>Time spent (hrs)</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
@@ -409,20 +410,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:G5"/>
+  <dimension ref="D4:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="7" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,10 +435,16 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -446,8 +454,29 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43365</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>10.25</v>
+      </c>
+      <c r="H6">
+        <v>12.5</v>
+      </c>
+      <c r="I6">
+        <f>H6-G6</f>
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>